<commit_message>
add branch sites, ancestral recon, scripts, and sepcies tree files
</commit_message>
<xml_diff>
--- a/metadata/transcriptome_sources.xlsx
+++ b/metadata/transcriptome_sources.xlsx
@@ -5,14 +5,14 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grovesdixon/gitreps/coral_reproductive_evolution/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grovesdixon/gitreps/coral_reproductive_evolution/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="2520" windowWidth="41380" windowHeight="22840" tabRatio="500"/>
+    <workbookView xWindow="6140" yWindow="4220" windowWidth="31060" windowHeight="19440" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="old" sheetId="1" r:id="rId1"/>
+    <sheet name="table" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
   <si>
     <t>Genus</t>
   </si>
@@ -273,12 +273,6 @@
     <t>http://www.ncbi.nlm.nih.gov/nuccore?LinkName=bioproject_nuccore&amp;from_uid=222758</t>
   </si>
   <si>
-    <t>Special Notes</t>
-  </si>
-  <si>
-    <t>Assembled from combination of A.cervicornis and A.palmata reads</t>
-  </si>
-  <si>
     <t>Libro et al. 2013</t>
   </si>
   <si>
@@ -303,36 +297,18 @@
     <t>https://peerj.com/articles/1616/#supplemental-information</t>
   </si>
   <si>
-    <t>citation title</t>
-  </si>
-  <si>
-    <t>RNA-Seq of the Caribbean reef-building coral Orbicella faveolata (Scleractinia-Merulinidae) under bleaching and disease stress expands models of coral innate immunity</t>
-  </si>
-  <si>
-    <t>Genomic basis for coral resilience to climate change</t>
-  </si>
-  <si>
     <t>Barshis et al. 2013</t>
   </si>
   <si>
     <t>http://palumbi.stanford.edu/data/</t>
   </si>
   <si>
-    <t>The genome of Aiptasia , a sea anemone model for coral symbiosis</t>
-  </si>
-  <si>
-    <t>Gene models from reference genome</t>
-  </si>
-  <si>
     <t>lobata</t>
   </si>
   <si>
     <t>australiensis</t>
   </si>
   <si>
-    <t>A snapshot of a coral "holobiont": A transcriptome assembly of the scleractinian coral, Porites, captures a wide variety of genes from both the host and symbiotic zooxanthellae</t>
-  </si>
-  <si>
     <t>https://www.ncbi.nlm.nih.gov/nuccore?term=236717%5BBioProject%5D</t>
   </si>
   <si>
@@ -360,41 +336,44 @@
     <t>https://www.dropbox.com/s/qvq3kus89aflyxf/Maqe.tar.gz?dl=0</t>
   </si>
   <si>
-    <t>this study</t>
+    <t>Galaxea</t>
+  </si>
+  <si>
+    <t>acrhelia</t>
+  </si>
+  <si>
+    <t>astreata</t>
+  </si>
+  <si>
+    <t>Goniopora</t>
+  </si>
+  <si>
+    <t>columna</t>
+  </si>
+  <si>
+    <t>Oculinidae</t>
+  </si>
+  <si>
+    <t>http://dornsife.usc.edu/labs/carlslab/data/</t>
   </si>
   <si>
     <t>capitata</t>
   </si>
   <si>
-    <t>columna</t>
-  </si>
-  <si>
-    <t>acrhelia</t>
-  </si>
-  <si>
-    <t>Galaxia</t>
-  </si>
-  <si>
-    <t>astreata</t>
-  </si>
-  <si>
-    <t>Goniopora</t>
-  </si>
-  <si>
-    <t>Euphylliidae</t>
-  </si>
-  <si>
-    <t>https://dornsife.usc.edu/labs/carlslab/data/</t>
-  </si>
-  <si>
-    <t>Broken link</t>
+    <t xml:space="preserve"> Frazier et al. 2017</t>
+  </si>
+  <si>
+    <t>ftp://ftp.ncbi.nlm.nih.gov/geo/series/GSE97nnn/GSE97888/suppl/GSE97888_Montiporacapitata_transcriptome.fasta.gz</t>
+  </si>
+  <si>
+    <t>Kenkel and Bay 2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -472,14 +451,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
@@ -531,7 +502,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -555,8 +526,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -566,12 +541,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -579,10 +551,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -594,6 +566,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -605,6 +579,8 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -939,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" zoomScalePageLayoutView="136" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -950,154 +926,152 @@
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="16" t="s">
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1108,20 +1082,16 @@
         <v>5</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1132,18 +1102,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1154,62 +1122,56 @@
         <v>5</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1220,130 +1182,116 @@
         <v>10</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1351,21 +1299,19 @@
         <v>21</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1373,234 +1319,196 @@
         <v>21</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="16" t="s">
+      <c r="D22" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="C26" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="H25" s="12"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="7" t="s">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="H26" s="12"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C27" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="7" t="s">
+      <c r="C28" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" s="12"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="F28" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>99</v>
+      <c r="E29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>